<commit_message>
minor changes to values
</commit_message>
<xml_diff>
--- a/Phase 2/Model Performance and Outputs/pre-trained_model_performance.xlsx
+++ b/Phase 2/Model Performance and Outputs/pre-trained_model_performance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Northeastern courses\DS 5500\Hurricane-Wind-Speed-Prediction-using-Deep-Learning-and-Machine-Learning\Phase 2\Model Performance and Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ARSH\NEU\Fall 2021\DS 5500\Project\Hurricane-Wind-Speed-Prediction-using-Deep-Learning-and-Machine-Learning\Phase 2\Model Performance and Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED75B5A-4B2A-471D-AA44-7BAFF15C2BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDB1872-1ACB-4AA6-B66E-8C349BE31CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12900" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0DA1A9-A4F4-4177-B619-9508B690AF05}"/>
+    <workbookView minimized="1" xWindow="132" yWindow="-312" windowWidth="21600" windowHeight="12672" xr2:uid="{0F0DA1A9-A4F4-4177-B619-9508B690AF05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Model Name</t>
   </si>
@@ -98,15 +98,6 @@
   </si>
   <si>
     <t>EfficientNet B7</t>
-  </si>
-  <si>
-    <t>366x367</t>
-  </si>
-  <si>
-    <t>366x368</t>
-  </si>
-  <si>
-    <t>366x369</t>
   </si>
   <si>
     <t>Train MSE</t>
@@ -464,7 +455,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -515,22 +506,22 @@
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.5">
@@ -744,7 +735,7 @@
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>12</v>
@@ -791,7 +782,7 @@
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>17</v>
@@ -838,7 +829,7 @@
         <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>18</v>

</xml_diff>